<commit_message>
swapped order to see if it makes a difference, it didn't
</commit_message>
<xml_diff>
--- a/r_script/cleaned_for_condorcet.xlsx
+++ b/r_script/cleaned_for_condorcet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamiesgro/Documents/code/dashboard/r_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3935FCC8-95A6-2746-BAE5-33E5965AE429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F40F9BB-FECC-2748-B6C1-7C98A274E2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21360" yWindow="2260" windowWidth="21360" windowHeight="15740" activeTab="6" xr2:uid="{A0F28E7B-37B7-2B47-A2D1-8B1DDFE71F8E}"/>
   </bookViews>
@@ -1396,7 +1396,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B5" activeCellId="1" sqref="A10:B11 A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1736,7 +1736,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>